<commit_message>
Updated Logger and Args
</commit_message>
<xml_diff>
--- a/hashtags.xlsx
+++ b/hashtags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florac/git/hashtag_selector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5312B08F-6CED-F340-93F3-305D33ACF064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE444E61-FC37-7942-A46D-26BE53D9DDF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16060" xr2:uid="{EA2F75E7-63ED-9B40-8936-7966021A97AE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="120">
   <si>
     <t>City</t>
   </si>
@@ -388,6 +388,12 @@
   </si>
   <si>
     <t>f87m2competition</t>
+  </si>
+  <si>
+    <t>repost</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -580,12 +586,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -600,9 +635,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,10 +648,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -628,6 +660,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F743E0-19EA-9E4A-B13E-7AFB3DA3CAD6}">
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection sqref="A1:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -969,1196 +1046,1341 @@
     <col min="17" max="17" width="13.1640625" customWidth="1"/>
     <col min="18" max="18" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21.1640625" customWidth="1"/>
+    <col min="20" max="23" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="14"/>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="15" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="14"/>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="15" t="s">
         <v>5</v>
       </c>
       <c r="M1" s="14"/>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="15" t="s">
         <v>6</v>
       </c>
       <c r="O1" s="14"/>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="15" t="s">
         <v>7</v>
       </c>
       <c r="Q1" s="14"/>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="17"/>
-      <c r="T1" s="13"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="23"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="16">
         <f>COUNTA(B4:B25)</f>
         <v>7</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15">
+      <c r="C2" s="11"/>
+      <c r="D2" s="16">
         <f t="shared" ref="D2:R2" si="0">COUNTA(D4:D25)</f>
         <v>17</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15">
+      <c r="E2" s="13"/>
+      <c r="F2" s="16">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15">
+      <c r="G2" s="13"/>
+      <c r="H2" s="16">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15">
+      <c r="I2" s="13"/>
+      <c r="J2" s="16">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15">
+        <v>19</v>
+      </c>
+      <c r="K2" s="13"/>
+      <c r="L2" s="16">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15">
+      <c r="M2" s="13"/>
+      <c r="N2" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15">
+      <c r="O2" s="13"/>
+      <c r="P2" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15">
+      <c r="Q2" s="13"/>
+      <c r="R2" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="S2" s="16"/>
-      <c r="T2" s="11">
+      <c r="S2" s="11"/>
+      <c r="T2" s="8">
         <f>SUM(B2:R2)</f>
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="9">
-        <f>ROUND(0.25*B2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="C3" s="9">
+      <c r="B3" s="17">
+        <f>ROUND($B$35*B$2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
         <f>SUM(C4:C24)</f>
         <v>1</v>
       </c>
-      <c r="D3" s="9">
-        <f t="shared" ref="D3:P3" si="1">ROUND(0.25*D2,0)</f>
-        <v>4</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="D3" s="17">
+        <f>ROUND($B$35*D$2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="7">
         <f>SUM(E4:E24)</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="F3" s="9">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="G3" s="9">
+      <c r="F3" s="17">
+        <f>ROUND($B$35*F$2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
         <f>SUM(G4:G24)</f>
         <v>6.5000000000000009</v>
       </c>
-      <c r="H3" s="9">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="I3" s="9">
+      <c r="H3" s="17">
+        <f>ROUND($B$35*H$2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="7">
         <f>SUM(I4:I24)</f>
         <v>10.600000000000003</v>
       </c>
-      <c r="J3" s="9">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="K3" s="9">
+      <c r="J3" s="17">
+        <f>ROUND($B$35*J$2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="K3" s="7">
         <f>SUM(K4:K24)</f>
-        <v>11.200000000000003</v>
-      </c>
-      <c r="L3" s="9">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="M3" s="9">
+        <v>12.200000000000003</v>
+      </c>
+      <c r="L3" s="17">
+        <f>ROUND($B$35*L$2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M3" s="7">
         <f>SUM(M4:M24)</f>
         <v>8.5</v>
       </c>
-      <c r="N3" s="9">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="O3" s="9">
+      <c r="N3" s="17">
+        <f>ROUND($B$35*N$2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="7">
         <f>SUM(O4:O24)</f>
         <v>5.1999999999999993</v>
       </c>
-      <c r="P3" s="9">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q3" s="9">
+      <c r="P3" s="17">
+        <f>ROUND($B$35*P$2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q3" s="7">
         <f>SUM(Q4:Q24)</f>
         <v>0.99999999999999978</v>
       </c>
-      <c r="R3" s="9">
-        <f>ROUND(0.25*R2,0)</f>
+      <c r="R3" s="17">
+        <f>ROUND($B$35*R$2,0)</f>
         <v>1</v>
       </c>
-      <c r="S3" s="10">
+      <c r="S3" s="6">
         <f>SUM(S4:S24)</f>
         <v>1</v>
       </c>
-      <c r="T3" s="12">
-        <f>SUM(B3:R3)</f>
-        <v>72</v>
+      <c r="T3" s="9">
+        <f>SUM(R3,P3,N3,L3,J3,H3,F3,D3,B3)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="20">
         <v>0.3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="19">
         <v>9.8039215686274522E-2</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="19">
         <v>0.9</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="19">
         <v>0.8</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="19">
         <v>1</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="19">
         <v>1</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="19">
         <v>0.8</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="19">
         <f>1/P$2</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="R4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="20">
         <f>1/R$2</f>
         <v>0.2</v>
       </c>
+      <c r="T4" s="24"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="20">
         <v>0.25</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="19">
         <v>9.8039215686274522E-2</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="19">
         <v>0.8</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="19">
         <v>0.7</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="19">
         <v>0.6</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="19">
         <v>0.7</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="2">
-        <f t="shared" ref="O5:O13" si="2">1/N$2</f>
+      <c r="O5" s="19">
+        <f t="shared" ref="O5:O13" si="1">1/N$2</f>
         <v>0.1</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" s="2">
-        <f t="shared" ref="Q5:Q10" si="3">1/P$2</f>
+      <c r="Q5" s="19">
+        <f t="shared" ref="Q5:Q10" si="2">1/P$2</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="R5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="S5" s="2">
-        <f t="shared" ref="S5:S8" si="4">1/R$2</f>
+      <c r="S5" s="20">
+        <f t="shared" ref="S5:S8" si="3">1/R$2</f>
         <v>0.2</v>
       </c>
+      <c r="T5" s="26"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="20">
         <v>0.15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="19">
         <v>9.8039215686274522E-2</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="19">
         <v>0.7</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="19">
         <v>0.6</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="19">
         <v>0.9</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="19">
         <v>0.7</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="19">
         <v>1</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="19">
+        <f t="shared" si="2"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="R6" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="S6" s="20">
         <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="T6" s="26"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="24"/>
+      <c r="B7" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="19">
+        <v>3.921568627450981E-2</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="19">
+        <v>1</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="N7" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" s="19">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q7" s="19">
+        <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="R6" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="S6" s="2">
-        <f t="shared" si="4"/>
+      <c r="R7" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="S7" s="20">
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="T7" s="26"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="24"/>
+      <c r="B8" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="20">
         <v>0.1</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D8" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="19">
         <v>3.921568627450981E-2</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="F8" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="19">
+        <v>0.9</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="19">
         <v>0.5</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="J8" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" s="19">
+        <v>0.9</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q8" s="19">
+        <f t="shared" si="2"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="R8" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="S8" s="20">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="T8" s="26"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="24"/>
+      <c r="B9" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="19">
+        <v>6.8627450980392163E-2</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="19">
+        <v>1</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O9" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q9" s="19">
+        <f t="shared" si="2"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="R9" s="18"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="26"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="19">
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" s="19">
+        <v>0.9</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="M10" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="O10" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q10" s="19">
+        <f t="shared" si="2"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="R10" s="18"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="26"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="19">
+        <v>6.8627450980392163E-2</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="N11" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="O11" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="26"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="24"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="19">
+        <v>8.8235294117647065E-2</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="M12" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="O12" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="26"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="24"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="19">
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="19">
         <v>0.4</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="2">
+      <c r="L13" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="O13" s="19">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="26"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="24"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="19">
+        <v>3.921568627450981E-2</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="19">
         <v>1</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" s="2">
+      <c r="L14" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="M14" s="19">
         <v>0.6</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" s="2">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q7" s="2">
-        <f t="shared" si="3"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="S7" s="2">
-        <f t="shared" si="4"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="N14" s="18"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="26"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="24"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="19">
+        <v>2.9411764705882353E-2</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="M15" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="N15" s="18"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="26"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="24"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="19">
+        <v>9.8039215686274522E-2</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="M16" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="N16" s="18"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="26"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="24"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="19">
+        <v>4.9019607843137261E-2</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I17" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="L17" s="18"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="26"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="19">
+        <v>1.9607843137254905E-2</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="K18" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="L18" s="18"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="26"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" s="24"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="19">
         <v>3.921568627450981E-2</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="2">
+      <c r="F19" s="18"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="19">
         <v>0.5</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O8" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q8" s="2">
-        <f t="shared" si="3"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="S8" s="2">
-        <f t="shared" si="4"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="2">
-        <v>6.8627450980392163E-2</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="2">
+      <c r="J19" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" s="19">
         <v>0.3</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="2">
+      <c r="L19" s="18"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="26"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" s="24"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="19">
+        <v>9.8039215686274526E-3</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="I20" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="K20" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="L20" s="18"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="26"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A21" s="24"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="K21" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="L21" s="18"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="26"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A22" s="24"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="K22" s="19">
         <v>1</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M9" s="2">
+      <c r="L22" s="18"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="26"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A23" s="24"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="J23" s="18"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="26"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A24" s="24"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" s="19">
         <v>0.5</v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q9" s="2">
-        <f t="shared" si="3"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="2">
-        <v>5.8823529411764705E-2</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q10" s="2">
-        <f t="shared" si="3"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="2">
-        <v>6.8627450980392163E-2</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="2">
-        <v>8.8235294117647065E-2</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M12" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="O12" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="2">
-        <v>5.8823529411764705E-2</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="O13" s="2">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="2">
-        <v>3.921568627450981E-2</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="M14" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2.9411764705882353E-2</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="M15" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="2">
-        <v>9.8039215686274522E-2</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="2">
-        <v>4.9019607843137261E-2</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1.9607843137254905E-2</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K18" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" s="2">
-        <v>3.921568627450981E-2</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="2">
-        <v>9.8039215686274526E-3</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K20" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="K21" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I24" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-    </row>
-    <row r="25" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J24" s="18"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="26"/>
+    </row>
+    <row r="25" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="27"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="26"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26" s="24"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="26"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A27" s="28"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="26"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="26"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A29" s="28"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="20"/>
+      <c r="T29" s="26"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" s="28"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="20"/>
+      <c r="T30" s="26"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" s="28"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="20"/>
+      <c r="T31" s="26"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="28"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="26"/>
+    </row>
+    <row r="33" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="31"/>
+      <c r="T33" s="9"/>
+    </row>
+    <row r="34" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
+    <row r="35" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="33">
+        <v>0.1</v>
+      </c>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="D1:E1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="R1:S1"/>
@@ -2172,6 +2394,11 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated Tag Creation Rules
</commit_message>
<xml_diff>
--- a/hashtags.xlsx
+++ b/hashtags.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florac/git/hashtag_selector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE444E61-FC37-7942-A46D-26BE53D9DDF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8D0386-08CF-F446-AB4E-14B0DEC12031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16060" xr2:uid="{EA2F75E7-63ED-9B40-8936-7966021A97AE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
   <si>
     <t>City</t>
   </si>
@@ -394,13 +394,31 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>#f80m3#f82m4#f87m2#m3#m4#m5#bmwnation#f8xgang#f8x#bmw_mpoweer#bmwmrepost#bmwrepost#bmw#bmwm#bmwm3#bmwm4#bmwm2#itswhitenoise#black_list#igbmw#clouds#carsofinstagram#bmwmbelgium#frontendfriday#m_town#carbon#carbonfiber#mperformance#bmw_world_ua#apollo_mlif3</t>
+  </si>
+  <si>
+    <t>bmwmrepost</t>
+  </si>
+  <si>
+    <t>black_list</t>
+  </si>
+  <si>
+    <t>igbmw</t>
+  </si>
+  <si>
+    <t>bmw_world_ua</t>
+  </si>
+  <si>
+    <t>apollo_mlif3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -426,6 +444,12 @@
     <font>
       <sz val="14"/>
       <color rgb="FF262626"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
@@ -620,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -648,24 +672,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -705,6 +711,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,7 +1048,7 @@
   <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD36"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1046,108 +1071,108 @@
     <col min="17" max="17" width="13.1640625" customWidth="1"/>
     <col min="18" max="18" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21.1640625" customWidth="1"/>
-    <col min="20" max="23" width="10.83203125" style="21"/>
+    <col min="20" max="23" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="15" t="s">
+      <c r="K1" s="34"/>
+      <c r="L1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="15" t="s">
+      <c r="M1" s="34"/>
+      <c r="N1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="15" t="s">
+      <c r="O1" s="34"/>
+      <c r="P1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="15" t="s">
+      <c r="Q1" s="34"/>
+      <c r="R1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="12"/>
-      <c r="T1" s="23"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="17"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="29">
         <f>COUNTA(B4:B25)</f>
         <v>7</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="16">
+      <c r="C2" s="30"/>
+      <c r="D2" s="29">
         <f t="shared" ref="D2:R2" si="0">COUNTA(D4:D25)</f>
         <v>17</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="16">
+      <c r="E2" s="33"/>
+      <c r="F2" s="29">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="16">
+      <c r="G2" s="33"/>
+      <c r="H2" s="29">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="16">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="16">
+      <c r="I2" s="33"/>
+      <c r="J2" s="29">
+        <f>COUNTA(J4:J26)</f>
+        <v>23</v>
+      </c>
+      <c r="K2" s="33"/>
+      <c r="L2" s="29">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="16">
+      <c r="M2" s="33"/>
+      <c r="N2" s="29">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="16">
+      <c r="O2" s="33"/>
+      <c r="P2" s="29">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="16">
+      <c r="Q2" s="33"/>
+      <c r="R2" s="29">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="S2" s="11"/>
+      <c r="S2" s="30"/>
       <c r="T2" s="8">
         <f>SUM(B2:R2)</f>
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="11">
         <f>ROUND($B$35*B$2,0)</f>
         <v>1</v>
       </c>
@@ -1155,55 +1180,55 @@
         <f>SUM(C4:C24)</f>
         <v>1</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="11">
         <f>ROUND($B$35*D$2,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="7">
         <f>SUM(E4:E24)</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="11">
         <f>ROUND($B$35*F$2,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="7">
         <f>SUM(G4:G24)</f>
         <v>6.5000000000000009</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="11">
         <f>ROUND($B$35*H$2,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I3" s="7">
         <f>SUM(I4:I24)</f>
         <v>10.600000000000003</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="11">
         <f>ROUND($B$35*J$2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="K3" s="7">
+        <f>SUM(K4:K27)</f>
+        <v>16</v>
+      </c>
+      <c r="L3" s="11">
+        <f>ROUND($B$35*L$2,0)</f>
         <v>2</v>
-      </c>
-      <c r="K3" s="7">
-        <f>SUM(K4:K24)</f>
-        <v>12.200000000000003</v>
-      </c>
-      <c r="L3" s="17">
-        <f>ROUND($B$35*L$2,0)</f>
-        <v>1</v>
       </c>
       <c r="M3" s="7">
         <f>SUM(M4:M24)</f>
         <v>8.5</v>
       </c>
-      <c r="N3" s="17">
+      <c r="N3" s="11">
         <f>ROUND($B$35*N$2,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O3" s="7">
         <f>SUM(O4:O24)</f>
         <v>5.1999999999999993</v>
       </c>
-      <c r="P3" s="17">
+      <c r="P3" s="11">
         <f>ROUND($B$35*P$2,0)</f>
         <v>1</v>
       </c>
@@ -1211,7 +1236,7 @@
         <f>SUM(Q4:Q24)</f>
         <v>0.99999999999999978</v>
       </c>
-      <c r="R3" s="17">
+      <c r="R3" s="11">
         <f>ROUND($B$35*R$2,0)</f>
         <v>1</v>
       </c>
@@ -1221,1114 +1246,1134 @@
       </c>
       <c r="T3" s="9">
         <f>SUM(R3,P3,N3,L3,J3,H3,F3,D3,B3)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
-      <c r="B4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="19">
+      <c r="E4" s="13">
         <v>9.8039215686274522E-2</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="13">
         <v>0.9</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="13">
         <v>0.8</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="13">
         <v>1</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="19">
+      <c r="M4" s="13">
         <v>1</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="19">
+      <c r="O4" s="13">
         <v>0.8</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="Q4" s="13">
         <f>1/P$2</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="R4" s="18" t="s">
+      <c r="R4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="20">
+      <c r="S4" s="14">
         <f>1/R$2</f>
         <v>0.2</v>
       </c>
-      <c r="T4" s="24"/>
+      <c r="T4" s="18"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="14">
         <v>0.25</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="13">
         <v>9.8039215686274522E-2</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="13">
         <v>0.8</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="13">
         <v>0.7</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="13">
         <v>0.6</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="13">
         <v>0.7</v>
       </c>
-      <c r="N5" s="18" t="s">
+      <c r="N5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="19">
+      <c r="O5" s="13">
         <f t="shared" ref="O5:O13" si="1">1/N$2</f>
         <v>0.1</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" s="19">
+      <c r="Q5" s="13">
         <f t="shared" ref="Q5:Q10" si="2">1/P$2</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="R5" s="18" t="s">
+      <c r="R5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="S5" s="20">
+      <c r="S5" s="14">
         <f t="shared" ref="S5:S8" si="3">1/R$2</f>
         <v>0.2</v>
       </c>
-      <c r="T5" s="26"/>
+      <c r="T5" s="20"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="14">
         <v>0.15</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="13">
         <v>9.8039215686274522E-2</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="13">
         <v>0.7</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="13">
         <v>0.6</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="13">
         <v>0.9</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="13">
         <v>0.7</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="19">
+      <c r="O6" s="13">
         <v>1</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="19">
+      <c r="Q6" s="13">
         <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="S6" s="20">
+      <c r="S6" s="14">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="T6" s="26"/>
+      <c r="T6" s="20"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
-      <c r="B7" s="18" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="14">
         <v>0.1</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="13">
         <v>3.921568627450981E-2</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="13">
         <v>0.5</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="13">
         <v>0.4</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="13">
         <v>1</v>
       </c>
-      <c r="L7" s="18" t="s">
+      <c r="L7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="13">
         <v>0.6</v>
       </c>
-      <c r="N7" s="18" t="s">
+      <c r="N7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="19">
+      <c r="O7" s="13">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="P7" s="18" t="s">
+      <c r="P7" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="Q7" s="19">
+      <c r="Q7" s="13">
         <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="R7" s="18" t="s">
+      <c r="R7" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="S7" s="20">
+      <c r="S7" s="14">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="T7" s="26"/>
+      <c r="T7" s="20"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="14">
         <v>0.1</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="13">
         <v>3.921568627450981E-2</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="13">
         <v>0.9</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="13">
         <v>0.5</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="13">
         <v>0.6</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="L8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="13">
         <v>0.9</v>
       </c>
-      <c r="N8" s="18" t="s">
+      <c r="N8" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="O8" s="19">
+      <c r="O8" s="13">
         <v>0.8</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="Q8" s="19">
+      <c r="Q8" s="13">
         <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="R8" s="18" t="s">
+      <c r="R8" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="S8" s="20">
+      <c r="S8" s="14">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="T8" s="26"/>
+      <c r="T8" s="20"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="14">
         <v>0.05</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="13">
         <v>6.8627450980392163E-2</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="13">
         <v>0.8</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="13">
         <v>0.3</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="13">
         <v>1</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="13">
         <v>0.5</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="13">
         <v>0.8</v>
       </c>
-      <c r="P9" s="18" t="s">
+      <c r="P9" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="Q9" s="19">
+      <c r="Q9" s="13">
         <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="R9" s="18"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="26"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="20"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="14">
         <v>0.05</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="13">
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="13">
         <v>0.7</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="13">
         <v>0.8</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="J10" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="13">
         <v>0.9</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="13">
         <v>0.5</v>
       </c>
-      <c r="N10" s="18" t="s">
+      <c r="N10" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="O10" s="19">
+      <c r="O10" s="13">
         <v>0.5</v>
       </c>
-      <c r="P10" s="18" t="s">
+      <c r="P10" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="Q10" s="19">
+      <c r="Q10" s="13">
         <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="R10" s="18"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="26"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="20"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="18" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="13">
         <v>6.8627450980392163E-2</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="13">
         <v>0.7</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="13">
         <v>0.2</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="J11" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="13">
         <v>0.5</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="M11" s="19">
+      <c r="M11" s="13">
         <v>0.5</v>
       </c>
-      <c r="N11" s="18" t="s">
+      <c r="N11" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="O11" s="19">
+      <c r="O11" s="13">
         <v>0.5</v>
       </c>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="26"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="20"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="18" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="13">
         <v>8.8235294117647065E-2</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="13">
         <v>0.5</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="13">
         <v>0.7</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="13">
         <v>0.5</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="L12" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="13">
         <v>0.5</v>
       </c>
-      <c r="N12" s="18" t="s">
+      <c r="N12" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="O12" s="19">
+      <c r="O12" s="13">
         <v>0.5</v>
       </c>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="26"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="20"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="18" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="13">
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="18" t="s">
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="13">
         <v>0.2</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="13">
         <v>0.4</v>
       </c>
-      <c r="L13" s="18" t="s">
+      <c r="L13" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="13">
         <v>0.6</v>
       </c>
-      <c r="N13" s="18" t="s">
+      <c r="N13" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="O13" s="19">
+      <c r="O13" s="13">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="26"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="20"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="18" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="13">
         <v>3.921568627450981E-2</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="18" t="s">
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="13">
         <v>0.7</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="13">
         <v>1</v>
       </c>
-      <c r="L14" s="18" t="s">
+      <c r="L14" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="13">
         <v>0.6</v>
       </c>
-      <c r="N14" s="18"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="26"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="20"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="18" t="s">
+      <c r="A15" s="18"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="13">
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="18" t="s">
+      <c r="F15" s="12"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="13">
         <v>0.8</v>
       </c>
-      <c r="J15" s="18" t="s">
+      <c r="J15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="13">
         <v>0.5</v>
       </c>
-      <c r="L15" s="18" t="s">
+      <c r="L15" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="M15" s="19">
+      <c r="M15" s="13">
         <v>0.6</v>
       </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="26"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="20"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="18" t="s">
+      <c r="A16" s="18"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="13">
         <v>9.8039215686274522E-2</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="18" t="s">
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="13">
         <v>0.5</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="J16" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="13">
         <v>0.4</v>
       </c>
-      <c r="L16" s="18" t="s">
+      <c r="L16" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="13">
         <v>0.8</v>
       </c>
-      <c r="N16" s="18"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="20"/>
-      <c r="T16" s="26"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="20"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="24"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="18" t="s">
+      <c r="A17" s="18"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="13">
         <v>4.9019607843137261E-2</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="18" t="s">
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="13">
         <v>0.5</v>
       </c>
-      <c r="J17" s="18" t="s">
+      <c r="J17" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="13">
         <v>0.6</v>
       </c>
-      <c r="L17" s="18"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="26"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="20"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="18" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="13">
         <v>1.9607843137254905E-2</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="18" t="s">
+      <c r="F18" s="12"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="13">
         <v>0.7</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="J18" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="13">
         <v>0.3</v>
       </c>
-      <c r="L18" s="18"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="26"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="20"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="18" t="s">
+      <c r="A19" s="18"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="13">
         <v>3.921568627450981E-2</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="18" t="s">
+      <c r="F19" s="12"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="13">
         <v>0.5</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="J19" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="13">
         <v>0.3</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="26"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="20"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="18" t="s">
+      <c r="A20" s="18"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="13">
         <v>9.8039215686274526E-3</v>
       </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="18" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="13">
         <v>0.3</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J20" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="K20" s="19">
+      <c r="K20" s="13">
         <v>0.3</v>
       </c>
-      <c r="L20" s="18"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="26"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="20"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="18" t="s">
+      <c r="A21" s="18"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="13">
         <v>0.3</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="J21" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="K21" s="19">
+      <c r="K21" s="13">
         <v>0.4</v>
       </c>
-      <c r="L21" s="18"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="26"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="20"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="18" t="s">
+      <c r="A22" s="18"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="13">
         <v>0.3</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="J22" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="K22" s="19">
+      <c r="K22" s="13">
         <v>1</v>
       </c>
-      <c r="L22" s="18"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="26"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="20"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="18" t="s">
+      <c r="A23" s="18"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="13">
         <v>0.3</v>
       </c>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="20"/>
-      <c r="T23" s="26"/>
+      <c r="J23" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="K23" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="L23" s="12"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="20"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="18" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="13">
         <v>0.5</v>
       </c>
-      <c r="J24" s="18"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="20"/>
-      <c r="T24" s="26"/>
+      <c r="J24" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="K24" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="L24" s="12"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="20"/>
     </row>
     <row r="25" spans="1:20" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="27"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="20"/>
-      <c r="T25" s="26"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="K25" s="13">
+        <v>1</v>
+      </c>
+      <c r="L25" s="12"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="20"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="24"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="26"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="K26" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="L26" s="12"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="20"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A27" s="28"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="26"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="K27" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="L27" s="12"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="20"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A28" s="24"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="20"/>
-      <c r="T28" s="26"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="20"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="28"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="20"/>
-      <c r="T29" s="26"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="14"/>
+      <c r="T29" s="20"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="28"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="20"/>
-      <c r="T30" s="26"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="20"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="20"/>
-      <c r="T31" s="26"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="20"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A32" s="28"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="20"/>
-      <c r="T32" s="26"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="20"/>
     </row>
     <row r="33" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="30"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="30"/>
-      <c r="S33" s="31"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="25"/>
       <c r="T33" s="9"/>
     </row>
     <row r="34" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2336,11 +2381,11 @@
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="33">
-        <v>0.1</v>
+      <c r="B35" s="27">
+        <v>0.18</v>
       </c>
       <c r="E35" s="2"/>
     </row>
@@ -2348,8 +2393,10 @@
       <c r="A36" s="5"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
+    <row r="37" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="28" t="s">
+        <v>120</v>
+      </c>
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
@@ -2381,13 +2428,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="D1:E1"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="N1:O1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B2:C2"/>
@@ -2395,10 +2440,12 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>